<commit_message>
implementirati paginator,sort i filtere
</commit_message>
<xml_diff>
--- a/SatiProcjeneOdrađenoGoranLolić.xlsx
+++ b/SatiProcjeneOdrađenoGoranLolić.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E475E2B-0F42-4107-9F99-93306652457D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BA1589-72E5-47AE-BDD7-BDD6FFFCFCFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8745" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,10 +225,10 @@
     <t>Realni odrađeni sati</t>
   </si>
   <si>
-    <t>2*</t>
-  </si>
-  <si>
     <t>* = Nedovršeno</t>
+  </si>
+  <si>
+    <t>7*</t>
   </si>
 </sst>
 </file>
@@ -769,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D4:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -1104,7 +1104,7 @@
         <v>10</v>
       </c>
       <c r="J32" s="21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -1456,7 +1456,7 @@
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
       <c r="J56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="4:10" ht="140.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Napravljene tablice za smještaje, prikaz podataka na frontendu
</commit_message>
<xml_diff>
--- a/SatiProcjeneOdrađenoGoranLolić.xlsx
+++ b/SatiProcjeneOdrađenoGoranLolić.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BA1589-72E5-47AE-BDD7-BDD6FFFCFCFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5F3125-B284-4E56-9293-75C8849761DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8745" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>PROJEKT XXXX</t>
   </si>
@@ -226,9 +226,6 @@
   </si>
   <si>
     <t>* = Nedovršeno</t>
-  </si>
-  <si>
-    <t>7*</t>
   </si>
 </sst>
 </file>
@@ -770,7 +767,7 @@
   <dimension ref="D4:P86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F16" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,8 +1100,8 @@
       <c r="I32">
         <v>10</v>
       </c>
-      <c r="J32" s="21" t="s">
-        <v>62</v>
+      <c r="J32" s="21">
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Dodan controller,mapper i service za gender i nationality
</commit_message>
<xml_diff>
--- a/SatiProcjeneOdrađenoGoranLolić.xlsx
+++ b/SatiProcjeneOdrađenoGoranLolić.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5F3125-B284-4E56-9293-75C8849761DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{713CF7A8-49EF-4441-B514-897C27A0F70D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8745" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8748" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE PROCJENE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>PROJEKT XXXX</t>
   </si>
@@ -226,6 +227,9 @@
   </si>
   <si>
     <t>* = Nedovršeno</t>
+  </si>
+  <si>
+    <t>2*</t>
   </si>
 </sst>
 </file>
@@ -767,21 +771,21 @@
   <dimension ref="D4:P86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F16" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="120.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="120.140625" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="120.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="120.109375" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E4" s="23" t="s">
         <v>0</v>
       </c>
@@ -797,7 +801,7 @@
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
     </row>
-    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
@@ -811,7 +815,7 @@
       <c r="O5" s="24"/>
       <c r="P5" s="24"/>
     </row>
-    <row r="9" spans="5:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="5:16" ht="21" x14ac:dyDescent="0.4">
       <c r="F9" s="17" t="s">
         <v>1</v>
       </c>
@@ -822,17 +826,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="5:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:16" ht="21" x14ac:dyDescent="0.4">
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" spans="5:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:16" ht="21" x14ac:dyDescent="0.4">
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="5:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:16" ht="18" x14ac:dyDescent="0.35">
       <c r="F12" s="13" t="s">
         <v>4</v>
       </c>
@@ -842,7 +846,7 @@
       </c>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="5:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:16" ht="18" x14ac:dyDescent="0.35">
       <c r="F13" s="13" t="s">
         <v>40</v>
       </c>
@@ -852,7 +856,7 @@
       </c>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="5:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:16" ht="18" x14ac:dyDescent="0.35">
       <c r="F14" s="13" t="s">
         <v>39</v>
       </c>
@@ -862,7 +866,7 @@
       </c>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="5:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="5:16" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F15" s="3" t="s">
         <v>5</v>
       </c>
@@ -872,13 +876,13 @@
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
       <c r="F17" s="25" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="25"/>
     </row>
-    <row r="18" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
@@ -898,7 +902,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E19" s="10" t="s">
         <v>11</v>
       </c>
@@ -915,7 +919,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E20" s="8"/>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -931,7 +935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
         <v>38</v>
       </c>
@@ -945,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E22" s="15" t="s">
         <v>14</v>
       </c>
@@ -961,7 +965,7 @@
       </c>
       <c r="J22" s="21"/>
     </row>
-    <row r="23" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E23" s="15" t="s">
         <v>15</v>
       </c>
@@ -979,7 +983,7 @@
       </c>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E24" s="15" t="s">
         <v>17</v>
       </c>
@@ -995,7 +999,7 @@
       </c>
       <c r="J24" s="21"/>
     </row>
-    <row r="25" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E25" s="11" t="s">
         <v>18</v>
       </c>
@@ -1008,13 +1012,13 @@
       </c>
       <c r="J25" s="21"/>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.3">
       <c r="J26" s="21"/>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.3">
       <c r="J27" s="21"/>
     </row>
-    <row r="28" spans="5:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:10" ht="21" x14ac:dyDescent="0.4">
       <c r="E28" s="2" t="s">
         <v>7</v>
       </c>
@@ -1032,7 +1036,7 @@
       </c>
       <c r="J28" s="21"/>
     </row>
-    <row r="29" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E29" s="10" t="s">
         <v>19</v>
       </c>
@@ -1052,7 +1056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E30" s="8"/>
       <c r="F30" s="5" t="s">
         <v>44</v>
@@ -1068,7 +1072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E31" s="4"/>
       <c r="F31" s="5" t="s">
         <v>41</v>
@@ -1086,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E32" s="4"/>
       <c r="F32" s="5" t="s">
         <v>41</v>
@@ -1104,7 +1108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E33" s="4"/>
       <c r="F33" s="5" t="s">
         <v>45</v>
@@ -1120,7 +1124,7 @@
       </c>
       <c r="J33" s="21"/>
     </row>
-    <row r="34" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E34" s="4"/>
       <c r="F34" s="5" t="s">
         <v>45</v>
@@ -1136,7 +1140,7 @@
       </c>
       <c r="J34" s="21"/>
     </row>
-    <row r="35" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E35" s="4"/>
       <c r="F35" s="5" t="s">
         <v>27</v>
@@ -1152,7 +1156,7 @@
       </c>
       <c r="J35" s="21"/>
     </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E36" s="9" t="s">
         <v>20</v>
       </c>
@@ -1168,7 +1172,7 @@
       </c>
       <c r="J36" s="21"/>
     </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E37" s="9" t="s">
         <v>15</v>
       </c>
@@ -1186,7 +1190,7 @@
       </c>
       <c r="J37" s="21"/>
     </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E38" s="9" t="s">
         <v>17</v>
       </c>
@@ -1202,7 +1206,7 @@
       </c>
       <c r="J38" s="21"/>
     </row>
-    <row r="39" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E39" s="11" t="s">
         <v>18</v>
       </c>
@@ -1215,13 +1219,13 @@
       </c>
       <c r="J39" s="21"/>
     </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:10" x14ac:dyDescent="0.3">
       <c r="J40" s="21"/>
     </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.3">
       <c r="J41" s="21"/>
     </row>
-    <row r="42" spans="5:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:10" ht="21" x14ac:dyDescent="0.4">
       <c r="E42" s="2" t="s">
         <v>7</v>
       </c>
@@ -1239,7 +1243,7 @@
       </c>
       <c r="J42" s="21"/>
     </row>
-    <row r="43" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E43" s="20" t="s">
         <v>30</v>
       </c>
@@ -1255,9 +1259,11 @@
       <c r="I43">
         <v>8</v>
       </c>
-      <c r="J43" s="21"/>
-    </row>
-    <row r="44" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J43" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E44" s="20"/>
       <c r="F44" t="s">
         <v>49</v>
@@ -1271,9 +1277,11 @@
       <c r="I44">
         <v>8</v>
       </c>
-      <c r="J44" s="21"/>
-    </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J44" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="5:10" x14ac:dyDescent="0.3">
       <c r="F45" t="s">
         <v>50</v>
       </c>
@@ -1286,9 +1294,11 @@
       <c r="I45">
         <v>8</v>
       </c>
-      <c r="J45" s="21"/>
-    </row>
-    <row r="46" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J45" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F46" s="5" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1313,7 @@
       </c>
       <c r="J46" s="21"/>
     </row>
-    <row r="47" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F47" s="5" t="s">
         <v>52</v>
       </c>
@@ -1318,7 +1328,7 @@
       </c>
       <c r="J47" s="21"/>
     </row>
-    <row r="48" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F48" s="5" t="s">
         <v>52</v>
       </c>
@@ -1333,7 +1343,7 @@
       </c>
       <c r="J48" s="21"/>
     </row>
-    <row r="49" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F49" s="5" t="s">
         <v>57</v>
       </c>
@@ -1348,7 +1358,7 @@
       </c>
       <c r="J49" s="21"/>
     </row>
-    <row r="50" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E50" s="4"/>
       <c r="F50" s="5" t="s">
         <v>33</v>
@@ -1364,7 +1374,7 @@
       </c>
       <c r="J50" s="21"/>
     </row>
-    <row r="51" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E51" s="4"/>
       <c r="F51" s="5" t="s">
         <v>35</v>
@@ -1380,7 +1390,7 @@
       </c>
       <c r="J51" s="21"/>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.3">
       <c r="E52" s="9" t="s">
         <v>20</v>
       </c>
@@ -1396,7 +1406,7 @@
       </c>
       <c r="J52" s="21"/>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:10" x14ac:dyDescent="0.3">
       <c r="E53" s="9" t="s">
         <v>15</v>
       </c>
@@ -1414,7 +1424,7 @@
       </c>
       <c r="J53" s="21"/>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:10" x14ac:dyDescent="0.3">
       <c r="E54" s="9" t="s">
         <v>17</v>
       </c>
@@ -1430,7 +1440,7 @@
       </c>
       <c r="J54" s="21"/>
     </row>
-    <row r="55" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E55" s="11" t="s">
         <v>18</v>
       </c>
@@ -1443,7 +1453,7 @@
       </c>
       <c r="J55" s="21"/>
     </row>
-    <row r="56" spans="4:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D56" s="4" t="s">
         <v>22</v>
       </c>
@@ -1456,25 +1466,25 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="4:10" ht="140.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:10" ht="140.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D57" s="4"/>
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
     </row>
-    <row r="58" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:10" ht="18" x14ac:dyDescent="0.35">
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:10" ht="18" x14ac:dyDescent="0.35">
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" spans="4:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D60" s="4"/>
       <c r="E60" s="22" t="s">
         <v>24</v>
@@ -1482,134 +1492,134 @@
       <c r="F60" s="22"/>
       <c r="G60" s="22"/>
     </row>
-    <row r="61" spans="4:10" ht="256.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:10" ht="256.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D61" s="4"/>
       <c r="E61" s="22"/>
       <c r="F61" s="22"/>
       <c r="G61" s="22"/>
     </row>
-    <row r="62" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:10" ht="18" x14ac:dyDescent="0.35">
       <c r="D62" s="4"/>
       <c r="E62" s="22"/>
       <c r="F62" s="22"/>
       <c r="G62" s="22"/>
     </row>
-    <row r="63" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:10" ht="18" x14ac:dyDescent="0.35">
       <c r="E64" s="4"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E65" s="4"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E66" s="4"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E67" s="4"/>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E68" s="4"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E69" s="4"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E70" s="4"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E71" s="4"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E72" s="4"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E73" s="4"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E74" s="4"/>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E75" s="4"/>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E76" s="4"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E77" s="4"/>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E78" s="4"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="79" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E79" s="4"/>
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="5:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="80" spans="5:7" ht="18" x14ac:dyDescent="0.35">
       <c r="E80" s="4"/>
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:9" ht="18" x14ac:dyDescent="0.35">
       <c r="E81" s="4"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:9" ht="18" x14ac:dyDescent="0.35">
       <c r="E82" s="4"/>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:9" ht="18" x14ac:dyDescent="0.35">
       <c r="E83" s="4"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:9" ht="18" x14ac:dyDescent="0.35">
       <c r="E84" s="4"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:9" ht="18" x14ac:dyDescent="0.35">
       <c r="E85" s="4"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:9" ht="18" x14ac:dyDescent="0.35">
       <c r="E86" s="7"/>
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>

</xml_diff>